<commit_message>
add % format data
</commit_message>
<xml_diff>
--- a/hello-apache-poi/helloPoiExcel.xlsx
+++ b/hello-apache-poi/helloPoiExcel.xlsx
@@ -12,21 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>姓名</t>
   </si>
   <si>
-    <t>性别</t>
-  </si>
-  <si>
-    <t>班级</t>
-  </si>
-  <si>
-    <t>数学</t>
-  </si>
-  <si>
-    <t>学费</t>
+    <t>文本</t>
+  </si>
+  <si>
+    <t>千分位数字</t>
+  </si>
+  <si>
+    <t>Double字段</t>
+  </si>
+  <si>
+    <t>数字文本混合</t>
+  </si>
+  <si>
+    <t>百分比</t>
   </si>
   <si>
     <t>Total
@@ -52,6 +55,9 @@
   </si>
   <si>
     <t>Indonesia</t>
+  </si>
+  <si>
+    <t>--</t>
   </si>
   <si>
     <t>M军</t>
@@ -94,19 +100,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,7 +124,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -128,13 +135,16 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1.37802E9</v>
@@ -145,13 +155,16 @@
       <c r="E2" t="n">
         <v>2016.0</v>
       </c>
+      <c r="F2" s="3" t="n">
+        <v>0.6812</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>3.23128E8</v>
@@ -160,15 +173,18 @@
         <v>35.32</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>2.5745300012E8</v>
@@ -179,13 +195,16 @@
       <c r="E4" t="n">
         <v>2016.0</v>
       </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>2.06081E8</v>
@@ -195,6 +214,29 @@
       </c>
       <c r="E5" t="n">
         <v>2016.0</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>2.0E-4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>2.06081E8</v>
+      </c>
+      <c r="D6" t="n">
+        <v>24.66</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2016.0</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>